<commit_message>
Se agregaron casi todos los campos para la matriz QC y todos de la hoja de hallazgos
Former-commit-id: 3948feb3ad6321c9327b13125596dbaca319f30c
</commit_message>
<xml_diff>
--- a/app/templates/bancolombia.xlsx
+++ b/app/templates/bancolombia.xlsx
@@ -5,26 +5,26 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="6" activeTab="18"/>
   </bookViews>
   <sheets>
-    <sheet name="Portada B" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Inicio" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Recursos" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="ToE" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="ToE (ACF)" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="CriterioFluid" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Portada B" sheetId="1" state="hidden" r:id="rId2"/>
+    <sheet name="Inicio" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Recursos" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="ToE" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="ToE (ACF)" sheetId="5" state="hidden" r:id="rId6"/>
+    <sheet name="CriterioFluid" sheetId="6" state="hidden" r:id="rId7"/>
     <sheet name="Hallazgos" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="CriterioBancolombia" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="CriterioBancolombia" sheetId="8" state="hidden" r:id="rId9"/>
     <sheet name="CriterioColpatria" sheetId="9" state="hidden" r:id="rId10"/>
     <sheet name="P_Ocurrencias" sheetId="10" state="hidden" r:id="rId11"/>
     <sheet name="P_General" sheetId="11" state="hidden" r:id="rId12"/>
     <sheet name="P_Cierre" sheetId="12" state="hidden" r:id="rId13"/>
     <sheet name="C_Activos" sheetId="13" state="hidden" r:id="rId14"/>
     <sheet name="CVSSv2" sheetId="14" state="hidden" r:id="rId15"/>
-    <sheet name="ActividadesPSI" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="ActividadesPSA" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="ActividadesACF" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="ActividadesPSI" sheetId="15" state="hidden" r:id="rId16"/>
+    <sheet name="ActividadesPSA" sheetId="16" state="hidden" r:id="rId17"/>
+    <sheet name="ActividadesACF" sheetId="17" state="hidden" r:id="rId18"/>
     <sheet name="CamposSeleccionQC" sheetId="18" state="hidden" r:id="rId19"/>
     <sheet name="MatrizQC" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
@@ -32,7 +32,11 @@
     <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">CriterioBancolombia!$A$2:$L$219</definedName>
     <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">CriterioColpatria!$D$2:$F$149</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">CriterioBancolombia!$A$2:$L$219</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">CriterioBancolombia!$A$2:$L$219</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">CriterioBancolombia!$A$2:$L$219</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">CriterioColpatria!$D$2:$F$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">CriterioColpatria!$D$2:$F$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">CriterioColpatria!$D$2:$F$149</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="AccessVecor" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -5818,7 +5822,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.###############"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -5933,7 +5937,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -5948,11 +5951,6 @@
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -5989,8 +5987,21 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -6255,7 +6266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6636,11 +6647,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6652,15 +6663,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6668,7 +6679,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6680,7 +6691,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6692,19 +6703,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6740,11 +6751,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6752,11 +6763,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6764,23 +6791,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6797,7 +6812,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -6816,34 +6831,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
       <border diagonalUp="false" diagonalDown="false">
@@ -8334,11 +8321,11 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubble3D val="0"/>
-        <c:axId val="50096510"/>
-        <c:axId val="87930252"/>
+        <c:axId val="3988053"/>
+        <c:axId val="54275447"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="50096510"/>
+        <c:axId val="3988053"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8380,12 +8367,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87930252"/>
+        <c:crossAx val="54275447"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87930252"/>
+        <c:axId val="54275447"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8418,7 +8405,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50096510"/>
+        <c:crossAx val="3988053"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8875,6 +8862,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -9038,6 +9026,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -9201,6 +9190,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -9342,11 +9332,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1154342"/>
-        <c:axId val="67957668"/>
+        <c:axId val="37854188"/>
+        <c:axId val="86387324"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1154342"/>
+        <c:axId val="37854188"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9417,14 +9407,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67957668"/>
+        <c:crossAx val="86387324"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67957668"/>
+        <c:axId val="86387324"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9504,7 +9494,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1154342"/>
+        <c:crossAx val="37854188"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9540,9 +9530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>894960</xdr:colOff>
+      <xdr:colOff>894240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9555,8 +9545,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2619360" y="438120"/>
-          <a:ext cx="2275920" cy="808920"/>
+          <a:off x="2543040" y="438120"/>
+          <a:ext cx="2199240" cy="808200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9577,9 +9567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1685520</xdr:colOff>
+      <xdr:colOff>1684800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9593,7 +9583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="771480" y="1790640"/>
-          <a:ext cx="5914440" cy="1371240"/>
+          <a:ext cx="5723280" cy="1370520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9627,9 +9617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>371160</xdr:colOff>
+      <xdr:colOff>370440</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9637,8 +9627,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2543040" y="7162560"/>
-        <a:ext cx="10038960" cy="5724360"/>
+        <a:off x="2447640" y="7162560"/>
+        <a:ext cx="9686160" cy="5723640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9662,9 +9652,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>4047840</xdr:colOff>
+      <xdr:colOff>4047120</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9672,8 +9662,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2828880" y="514440"/>
-        <a:ext cx="6038280" cy="3999960"/>
+        <a:off x="2714760" y="514440"/>
+        <a:ext cx="5961240" cy="3999240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9697,9 +9687,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>380520</xdr:colOff>
+      <xdr:colOff>379800</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>199800</xdr:rowOff>
+      <xdr:rowOff>199080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9707,8 +9697,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4514400" y="1199880"/>
-        <a:ext cx="6171840" cy="4000320"/>
+        <a:off x="4381200" y="1199880"/>
+        <a:ext cx="5961600" cy="3999600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9732,9 +9722,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>609120</xdr:colOff>
+      <xdr:colOff>608400</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9742,8 +9732,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8076960" y="3657600"/>
-        <a:ext cx="10153080" cy="4095000"/>
+        <a:off x="7752960" y="3657600"/>
+        <a:ext cx="9800280" cy="4094280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9770,15 +9760,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="str">
         <f aca="false">"Documentación " &amp; Inicio!B7 &amp;  " " &amp; "- " &amp; Inicio!B6</f>
-        <v>Documentación Pruebas Integrales [PI] - </v>
+        <v>Documentación Pruebas Integrales [PI] -</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -9850,14 +9840,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="13.6326530612245"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11438,11 +11428,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.6836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11520,16 +11510,16 @@
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.4336734693878"/>
     <col collapsed="false" hidden="true" max="8" min="7" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12337,25 +12327,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.29591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.80612244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="5.80612244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="5.80612244897959"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="21" min="18" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="2.42857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.02551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="18" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15173,13 +15163,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.56632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15835,14 +15826,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16549,14 +16540,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.6224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17008,13 +16999,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.484693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.7295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17672,16 +17663,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18812,56 +18803,56 @@
   </sheetPr>
   <dimension ref="A1:AR31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="49.2704081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="59.8010204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="46.3010204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="40.5"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="43.3316326530612"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="49.8112244897959"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="58.4489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.9489795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="45.2244897959184"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="48.7295918367347"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="34.9642857142857"/>
     <col collapsed="false" hidden="true" max="44" min="44" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19092,13 +19083,13 @@
       </c>
       <c r="AR2" s="128"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="87" t="s">
         <v>1736</v>
       </c>
-      <c r="B3" s="87"/>
+      <c r="B3" s="131"/>
       <c r="C3" s="87"/>
-      <c r="D3" s="131"/>
+      <c r="D3" s="132"/>
       <c r="E3" s="87"/>
       <c r="F3" s="87" t="n">
         <f aca="false">Inicio!$B$6</f>
@@ -19111,8 +19102,7 @@
         <v>REQ.0001 El mecanismo de administración de un sistema, debe ser accesible solo desde segmentos de red de gestión o administrativos.
 (Capa:Capa de Aplicación, Alcance:Confidencialidad, Activo:Administración del sistema, Fase:Operación)
 REQ.0002 Los activos de información del sistema deben estar identificados.
-(Capa:Capa de Recursos, Alcance:Adherencia, Activo:Activos de información, Fase:Análisis)
-</v>
+(Capa:Capa de Recursos, Alcance:Adherencia, Activo:Activos de información, Fase:Análisis)</v>
       </c>
       <c r="J3" s="87" t="s">
         <v>1483</v>
@@ -19160,7 +19150,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W3" s="132" t="n">
+      <c r="W3" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR3)</f>
         <v>10</v>
       </c>
@@ -19248,8 +19238,7 @@
       <c r="I4" s="87" t="str">
         <f aca="true">INDIRECT("Hallazgos!E"&amp;AR4)</f>
         <v>REQ.0050 Los eventos con severidad de depuración no deben estar habilitados en producción.
-(Capa:Capa de Aplicación, Alcance:Confidencialidad, Activo:Bitácoras, Fase:Operación)
-</v>
+(Capa:Capa de Aplicación, Alcance:Confidencialidad, Activo:Bitácoras, Fase:Operación)</v>
       </c>
       <c r="J4" s="87" t="str">
         <f aca="false">J3</f>
@@ -19300,7 +19289,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W4" s="132" t="n">
+      <c r="W4" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR4)</f>
         <v>10</v>
       </c>
@@ -19391,8 +19380,7 @@
       <c r="I5" s="87" t="str">
         <f aca="true">INDIRECT("Hallazgos!E"&amp;AR5)</f>
         <v>REQ.0250 La aplicación debe garantizar que las peticiones que reciba a recursos no sigan un patrón discernible.
-(Capa:Capa de Aplicación, Alcance:Madurez, Activo:Código fuente, Fase:Construcción)
-</v>
+(Capa:Capa de Aplicación, Alcance:Madurez, Activo:Código fuente, Fase:Construcción)</v>
       </c>
       <c r="J5" s="87" t="str">
         <f aca="false">J4</f>
@@ -19443,7 +19431,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W5" s="132" t="n">
+      <c r="W5" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR5)</f>
         <v>10</v>
       </c>
@@ -19534,8 +19522,7 @@
       <c r="I6" s="87" t="str">
         <f aca="true">INDIRECT("Hallazgos!E"&amp;AR6)</f>
         <v>REQ.0040 El sistema debe requerir autenticación para todos los recursos, excepto para aquellos específicamente clasificados como públicos.
-(Capa:Capa de Aplicación, Alcance:Autorización, Activo:Recursos del sistema, Fase:Operación)
-</v>
+(Capa:Capa de Aplicación, Alcance:Autorización, Activo:Recursos del sistema, Fase:Operación)</v>
       </c>
       <c r="J6" s="87" t="str">
         <f aca="false">J5</f>
@@ -19586,7 +19573,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W6" s="132" t="n">
+      <c r="W6" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR6)</f>
         <v>10</v>
       </c>
@@ -19727,7 +19714,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W7" s="132" t="n">
+      <c r="W7" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR7)</f>
         <v>10</v>
       </c>
@@ -19868,7 +19855,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W8" s="132" t="n">
+      <c r="W8" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR8)</f>
         <v>10</v>
       </c>
@@ -20009,7 +19996,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W9" s="132" t="n">
+      <c r="W9" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR9)</f>
         <v>10</v>
       </c>
@@ -20150,7 +20137,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W10" s="132" t="n">
+      <c r="W10" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR10)</f>
         <v>10</v>
       </c>
@@ -20291,7 +20278,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W11" s="132" t="n">
+      <c r="W11" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR11)</f>
         <v>10</v>
       </c>
@@ -20432,7 +20419,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W12" s="132" t="n">
+      <c r="W12" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR12)</f>
         <v>10</v>
       </c>
@@ -20573,7 +20560,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W13" s="132" t="n">
+      <c r="W13" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR13)</f>
         <v>10</v>
       </c>
@@ -20714,7 +20701,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W14" s="132" t="n">
+      <c r="W14" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR14)</f>
         <v>10</v>
       </c>
@@ -20855,7 +20842,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W15" s="132" t="n">
+      <c r="W15" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR15)</f>
         <v>10</v>
       </c>
@@ -20996,7 +20983,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W16" s="132" t="n">
+      <c r="W16" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR16)</f>
         <v>10</v>
       </c>
@@ -21137,7 +21124,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W17" s="132" t="n">
+      <c r="W17" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR17)</f>
         <v>10</v>
       </c>
@@ -21278,7 +21265,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W18" s="132" t="n">
+      <c r="W18" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR18)</f>
         <v>10</v>
       </c>
@@ -21419,7 +21406,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W19" s="132" t="n">
+      <c r="W19" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR19)</f>
         <v>10</v>
       </c>
@@ -21560,7 +21547,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W20" s="132" t="n">
+      <c r="W20" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR20)</f>
         <v>10</v>
       </c>
@@ -21701,7 +21688,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W21" s="132" t="n">
+      <c r="W21" s="133" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR21)</f>
         <v>10</v>
       </c>
@@ -23189,9 +23176,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="52.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="51.5663265306123"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23446,10 +23433,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23586,12 +23573,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23875,12 +23862,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24130,18 +24117,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.9693877551021"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
     <col collapsed="false" hidden="true" max="11" min="11" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35192,27 +35179,27 @@
   </sheetPr>
   <dimension ref="A1:O192"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35298,8 +35285,7 @@
         <v>REQ.0001 El mecanismo de administración de un sistema, debe ser accesible solo desde segmentos de red de gestión o administrativos.
 (Capa:Capa de Aplicación, Alcance:Confidencialidad, Activo:Administración del sistema, Fase:Operación)
 REQ.0002 Los activos de información del sistema deben estar identificados.
-(Capa:Capa de Recursos, Alcance:Adherencia, Activo:Activos de información, Fase:Análisis)
-</v>
+(Capa:Capa de Recursos, Alcance:Adherencia, Activo:Activos de información, Fase:Análisis)</v>
       </c>
       <c r="F3" s="50" t="str">
         <f aca="false">CVSSv2!$A$4</f>
@@ -35528,7 +35514,7 @@
       <c r="N12" s="52"/>
       <c r="O12" s="52"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="n">
         <f aca="false">IF(A12="#",1,A3+1)</f>
         <v>2</v>
@@ -35536,15 +35522,14 @@
       <c r="B13" s="18" t="s">
         <v>742</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="18"/>
       <c r="E13" s="18" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("CONCATENATE(ARRAYFORMULA(QUERY(QUERY(Indirect(C_Activos!$L$1&amp;""!A:F""),""SELECT A, B, C, D, E, F WHERE A MATCHES '""&amp;M13&amp;""'""),""select Col1"")&amp;"" ""&amp;QUERY(QUERY(Indirect(C_Activos!$L$1&amp;""!A:F""),""SELECT A, B, C, D, E, F WHERE A MATCHES '""&amp;M13&amp;""'""),""select Col2"")&amp;CHAR(10)&amp;""(Capa:""&amp;QUERY(QUERY(Indirect(C_Activos!$L$1&amp;""!A:F""),""SELECT A, B, C, D, E, F WHERE A MATCHES '""&amp;M13&amp;""'""),""select Col3"")&amp;"", Alcance:""&amp;QUERY(QUERY(Indirect(C_Activos!$L$1&amp;""!A:F""),""SELECT A, B, C, D, E, F WHERE A MATCHES '""&amp;M13&amp;""'""),""select Col5"")&amp;"", Activo:""&amp;QUERY(QUERY(Indirect(C_Activos!$L$1&amp;""!A:F""),""SELECT A, B, C, D, E, F WHERE A MATCHES '""&amp;M13&amp;""'""),""select Col4"")&amp;"", Fase:""&amp;QUERY(QUERY(Indirect(C_Activos!$L$1&amp;""!A:F""),""SELECT A, B, C, D, E, F WHERE A MATCHES '""&amp;M13&amp;""'""),""select Col6"")&amp;"")""&amp;CHAR(10)&amp;CHAR(10)))"),"REQ.0050 Los eventos con severidad de depuración no deben estar habilitados en producción.
 (Capa:Capa de Aplicación, Alcance:Confidencialidad, Activo:Bitácoras, Fase:Operación)
 ")</f>
         <v>REQ.0050 Los eventos con severidad de depuración no deben estar habilitados en producción.
-(Capa:Capa de Aplicación, Alcance:Confidencialidad, Activo:Bitácoras, Fase:Operación)
-</v>
+(Capa:Capa de Aplicación, Alcance:Confidencialidad, Activo:Bitácoras, Fase:Operación)</v>
       </c>
       <c r="F13" s="50" t="str">
         <f aca="false">CVSSv2!$A$4</f>
@@ -35788,8 +35773,7 @@
 (Capa:Capa de Aplicación, Alcance:Madurez, Activo:Código fuente, Fase:Construcción)
 ")</f>
         <v>REQ.0250 La aplicación debe garantizar que las peticiones que reciba a recursos no sigan un patrón discernible.
-(Capa:Capa de Aplicación, Alcance:Madurez, Activo:Código fuente, Fase:Construcción)
-</v>
+(Capa:Capa de Aplicación, Alcance:Madurez, Activo:Código fuente, Fase:Construcción)</v>
       </c>
       <c r="F23" s="50" t="str">
         <f aca="false">CVSSv2!$A$4</f>
@@ -36031,8 +36015,7 @@
 (Capa:Capa de Aplicación, Alcance:Autorización, Activo:Recursos del sistema, Fase:Operación)
 ")</f>
         <v>REQ.0040 El sistema debe requerir autenticación para todos los recursos, excepto para aquellos específicamente clasificados como públicos.
-(Capa:Capa de Aplicación, Alcance:Autorización, Activo:Recursos del sistema, Fase:Operación)
-</v>
+(Capa:Capa de Aplicación, Alcance:Autorización, Activo:Recursos del sistema, Fase:Operación)</v>
       </c>
       <c r="F33" s="50" t="str">
         <f aca="false">CVSSv2!$A$4</f>
@@ -40490,15 +40473,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.4234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="49"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="81.5357142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="47.7857142857143"/>
     <col collapsed="false" hidden="true" max="12" min="12" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49583,15 +49566,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="68.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="66.9540816326531"/>
     <col collapsed="false" hidden="true" max="8" min="8" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Se borro todos los archivos pyc y se agrego la condicion al git ignore, se ocultaron los campos innecesarios del template tecnico de bancolombia
Former-commit-id: 019c2c3992f1fe0b8b696b47aabbd9bfaea5dc49
</commit_message>
<xml_diff>
--- a/app/templates/bancolombia.xlsx
+++ b/app/templates/bancolombia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="6" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Portada B" sheetId="1" state="hidden" r:id="rId2"/>
@@ -34,9 +34,11 @@
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">CriterioBancolombia!$A$2:$L$219</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">CriterioBancolombia!$A$2:$L$219</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">CriterioBancolombia!$A$2:$L$219</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">CriterioBancolombia!$A$2:$L$219</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">CriterioColpatria!$D$2:$F$149</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">CriterioColpatria!$D$2:$F$149</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">CriterioColpatria!$D$2:$F$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">CriterioColpatria!$D$2:$F$149</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="AccessVecor" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -6266,7 +6268,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6787,8 +6789,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="28" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -6905,7 +6915,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8321,11 +8331,11 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubble3D val="0"/>
-        <c:axId val="3988053"/>
-        <c:axId val="54275447"/>
+        <c:axId val="13034837"/>
+        <c:axId val="38594342"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="3988053"/>
+        <c:axId val="13034837"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8367,12 +8377,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54275447"/>
+        <c:crossAx val="38594342"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54275447"/>
+        <c:axId val="38594342"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8405,7 +8415,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3988053"/>
+        <c:crossAx val="13034837"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8438,7 +8448,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8645,7 +8655,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8828,7 +8838,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9332,11 +9342,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="37854188"/>
-        <c:axId val="86387324"/>
+        <c:axId val="32587105"/>
+        <c:axId val="27164820"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="37854188"/>
+        <c:axId val="32587105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9407,14 +9417,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86387324"/>
+        <c:crossAx val="27164820"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86387324"/>
+        <c:axId val="27164820"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9494,7 +9504,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37854188"/>
+        <c:crossAx val="32587105"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9530,9 +9540,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>894240</xdr:colOff>
+      <xdr:colOff>893880</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9545,8 +9555,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2543040" y="438120"/>
-          <a:ext cx="2199240" cy="808200"/>
+          <a:off x="2504880" y="438120"/>
+          <a:ext cx="2160720" cy="807840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9567,9 +9577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1684800</xdr:colOff>
+      <xdr:colOff>1684440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9583,7 +9593,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="771480" y="1790640"/>
-          <a:ext cx="5723280" cy="1370520"/>
+          <a:ext cx="5627520" cy="1370160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9617,9 +9627,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>370440</xdr:colOff>
+      <xdr:colOff>370080</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9627,8 +9637,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2447640" y="7162560"/>
-        <a:ext cx="9686160" cy="5723640"/>
+        <a:off x="2400120" y="7162560"/>
+        <a:ext cx="9504720" cy="5723280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9652,9 +9662,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>4047120</xdr:colOff>
+      <xdr:colOff>4046760</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9662,8 +9672,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2714760" y="514440"/>
-        <a:ext cx="5961240" cy="3999240"/>
+        <a:off x="2657520" y="514440"/>
+        <a:ext cx="5923080" cy="3998880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9687,9 +9697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>379800</xdr:colOff>
+      <xdr:colOff>379440</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>199080</xdr:rowOff>
+      <xdr:rowOff>198720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9697,8 +9707,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4381200" y="1199880"/>
-        <a:ext cx="5961600" cy="3999600"/>
+        <a:off x="4314600" y="1199880"/>
+        <a:ext cx="5865840" cy="3999240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9722,9 +9732,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>608400</xdr:colOff>
+      <xdr:colOff>608040</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9732,8 +9742,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7752960" y="3657600"/>
-        <a:ext cx="9800280" cy="4094280"/>
+        <a:off x="7581600" y="3657600"/>
+        <a:ext cx="9618840" cy="4093920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9760,9 +9770,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9840,14 +9850,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="13.3622448979592"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11428,11 +11438,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="64.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11510,16 +11520,16 @@
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1632653061224"/>
     <col collapsed="false" hidden="true" max="8" min="7" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12327,25 +12337,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.02551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="47.9234693877551"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="21" min="18" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="1.88775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="47.2448979591837"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="21" min="18" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="2.02551020408163"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15163,14 +15173,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.29591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15826,14 +15836,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.7295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16540,14 +16550,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.6224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.6734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16999,13 +17009,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.7295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.7857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17663,16 +17673,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18803,59 +18813,52 @@
   </sheetPr>
   <dimension ref="A1:AR31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BI2" activeCellId="0" sqref="BI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="48.1938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="58.4489795918367"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.9489795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="45.2244897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="48.7295918367347"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="true" max="44" min="44" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="true" max="4" min="1" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="true" max="7" min="7" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="true" max="10" min="10" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="true" max="12" min="12" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="57.7755102040816"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.4081632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="44.6836734693878"/>
+    <col collapsed="false" hidden="true" max="21" min="20" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="true" max="33" min="31" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="true" max="35" min="35" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="true" max="39" min="38" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="true" max="60" min="44" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="1025" min="61" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="124"/>
       <c r="B1" s="125" t="s">
         <v>1706</v>
@@ -18951,7 +18954,7 @@
       </c>
       <c r="AR1" s="125"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="129" t="s">
         <v>1710</v>
       </c>
@@ -18964,121 +18967,121 @@
       <c r="D2" s="129" t="s">
         <v>1456</v>
       </c>
-      <c r="E2" s="128" t="s">
+      <c r="E2" s="130" t="s">
         <v>1457</v>
       </c>
-      <c r="F2" s="130" t="s">
+      <c r="F2" s="131" t="s">
         <v>1712</v>
       </c>
-      <c r="G2" s="129" t="s">
+      <c r="G2" s="132" t="s">
         <v>1713</v>
       </c>
-      <c r="H2" s="128" t="s">
+      <c r="H2" s="130" t="s">
         <v>1714</v>
       </c>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="131" t="s">
         <v>1715</v>
       </c>
-      <c r="J2" s="128" t="s">
+      <c r="J2" s="130" t="s">
         <v>1716</v>
       </c>
-      <c r="K2" s="128" t="s">
+      <c r="K2" s="130" t="s">
         <v>1717</v>
       </c>
-      <c r="L2" s="129" t="s">
+      <c r="L2" s="132" t="s">
         <v>1459</v>
       </c>
-      <c r="M2" s="128" t="s">
+      <c r="M2" s="130" t="s">
         <v>1460</v>
       </c>
-      <c r="N2" s="130" t="s">
+      <c r="N2" s="131" t="s">
         <v>717</v>
       </c>
-      <c r="O2" s="130" t="s">
+      <c r="O2" s="131" t="s">
         <v>1718</v>
       </c>
-      <c r="P2" s="130" t="s">
+      <c r="P2" s="131" t="s">
         <v>718</v>
       </c>
-      <c r="Q2" s="128" t="s">
+      <c r="Q2" s="130" t="s">
         <v>1461</v>
       </c>
-      <c r="R2" s="128" t="s">
+      <c r="R2" s="130" t="s">
         <v>1719</v>
       </c>
-      <c r="S2" s="128" t="s">
+      <c r="S2" s="130" t="s">
         <v>1720</v>
       </c>
-      <c r="T2" s="128" t="s">
+      <c r="T2" s="130" t="s">
         <v>1463</v>
       </c>
-      <c r="U2" s="128" t="s">
+      <c r="U2" s="130" t="s">
         <v>1721</v>
       </c>
-      <c r="V2" s="130" t="s">
+      <c r="V2" s="131" t="s">
         <v>720</v>
       </c>
-      <c r="W2" s="130" t="s">
+      <c r="W2" s="131" t="s">
         <v>1722</v>
       </c>
-      <c r="X2" s="130" t="s">
+      <c r="X2" s="131" t="s">
         <v>1723</v>
       </c>
-      <c r="Y2" s="130" t="s">
+      <c r="Y2" s="131" t="s">
         <v>722</v>
       </c>
-      <c r="Z2" s="128" t="s">
+      <c r="Z2" s="130" t="s">
         <v>1724</v>
       </c>
-      <c r="AA2" s="128" t="s">
+      <c r="AA2" s="130" t="s">
         <v>1464</v>
       </c>
-      <c r="AB2" s="130" t="s">
+      <c r="AB2" s="131" t="s">
         <v>1725</v>
       </c>
-      <c r="AC2" s="130" t="s">
+      <c r="AC2" s="131" t="s">
         <v>1726</v>
       </c>
-      <c r="AD2" s="128" t="s">
+      <c r="AD2" s="130" t="s">
         <v>1727</v>
       </c>
-      <c r="AE2" s="129" t="s">
+      <c r="AE2" s="132" t="s">
         <v>1728</v>
       </c>
-      <c r="AF2" s="128" t="s">
+      <c r="AF2" s="130" t="s">
         <v>1729</v>
       </c>
-      <c r="AG2" s="128" t="s">
+      <c r="AG2" s="130" t="s">
         <v>1730</v>
       </c>
-      <c r="AH2" s="128" t="s">
+      <c r="AH2" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="128" t="s">
+      <c r="AI2" s="130" t="s">
         <v>1731</v>
       </c>
-      <c r="AJ2" s="128" t="s">
+      <c r="AJ2" s="130" t="s">
         <v>1732</v>
       </c>
-      <c r="AK2" s="128" t="s">
+      <c r="AK2" s="130" t="s">
         <v>1733</v>
       </c>
-      <c r="AL2" s="128" t="s">
+      <c r="AL2" s="130" t="s">
         <v>1734</v>
       </c>
-      <c r="AM2" s="128" t="s">
+      <c r="AM2" s="130" t="s">
         <v>1735</v>
       </c>
-      <c r="AN2" s="128" t="s">
+      <c r="AN2" s="130" t="s">
         <v>1467</v>
       </c>
-      <c r="AO2" s="130" t="s">
+      <c r="AO2" s="131" t="s">
         <v>723</v>
       </c>
-      <c r="AP2" s="130" t="s">
+      <c r="AP2" s="131" t="s">
         <v>724</v>
       </c>
-      <c r="AQ2" s="130" t="s">
+      <c r="AQ2" s="131" t="s">
         <v>725</v>
       </c>
       <c r="AR2" s="128"/>
@@ -19087,9 +19090,9 @@
       <c r="A3" s="87" t="s">
         <v>1736</v>
       </c>
-      <c r="B3" s="131"/>
+      <c r="B3" s="133"/>
       <c r="C3" s="87"/>
-      <c r="D3" s="132"/>
+      <c r="D3" s="134"/>
       <c r="E3" s="87"/>
       <c r="F3" s="87" t="n">
         <f aca="false">Inicio!$B$6</f>
@@ -19150,7 +19153,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W3" s="133" t="n">
+      <c r="W3" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR3)</f>
         <v>10</v>
       </c>
@@ -19208,7 +19211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="87" t="str">
         <f aca="false">A3</f>
         <v>Ruta en QC</v>
@@ -19289,7 +19292,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W4" s="133" t="n">
+      <c r="W4" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR4)</f>
         <v>10</v>
       </c>
@@ -19350,7 +19353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="87" t="str">
         <f aca="false">A4</f>
         <v>Ruta en QC</v>
@@ -19431,7 +19434,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W5" s="133" t="n">
+      <c r="W5" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR5)</f>
         <v>10</v>
       </c>
@@ -19492,7 +19495,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="87" t="str">
         <f aca="false">A5</f>
         <v>Ruta en QC</v>
@@ -19573,7 +19576,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W6" s="133" t="n">
+      <c r="W6" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR6)</f>
         <v>10</v>
       </c>
@@ -19634,7 +19637,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="87" t="str">
         <f aca="false">A6</f>
         <v>Ruta en QC</v>
@@ -19714,7 +19717,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W7" s="133" t="n">
+      <c r="W7" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR7)</f>
         <v>10</v>
       </c>
@@ -19775,7 +19778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="87" t="str">
         <f aca="false">A7</f>
         <v>Ruta en QC</v>
@@ -19855,7 +19858,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W8" s="133" t="n">
+      <c r="W8" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR8)</f>
         <v>10</v>
       </c>
@@ -19916,7 +19919,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="87" t="str">
         <f aca="false">A8</f>
         <v>Ruta en QC</v>
@@ -19996,7 +19999,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W9" s="133" t="n">
+      <c r="W9" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR9)</f>
         <v>10</v>
       </c>
@@ -20057,7 +20060,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="87" t="str">
         <f aca="false">A9</f>
         <v>Ruta en QC</v>
@@ -20137,7 +20140,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W10" s="133" t="n">
+      <c r="W10" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR10)</f>
         <v>10</v>
       </c>
@@ -20198,7 +20201,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="87" t="str">
         <f aca="false">A10</f>
         <v>Ruta en QC</v>
@@ -20278,7 +20281,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W11" s="133" t="n">
+      <c r="W11" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR11)</f>
         <v>10</v>
       </c>
@@ -20339,7 +20342,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="87" t="str">
         <f aca="false">A11</f>
         <v>Ruta en QC</v>
@@ -20419,7 +20422,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W12" s="133" t="n">
+      <c r="W12" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR12)</f>
         <v>10</v>
       </c>
@@ -20480,7 +20483,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="87" t="str">
         <f aca="false">A12</f>
         <v>Ruta en QC</v>
@@ -20560,7 +20563,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W13" s="133" t="n">
+      <c r="W13" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR13)</f>
         <v>10</v>
       </c>
@@ -20621,7 +20624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="87" t="str">
         <f aca="false">A13</f>
         <v>Ruta en QC</v>
@@ -20701,7 +20704,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W14" s="133" t="n">
+      <c r="W14" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR14)</f>
         <v>10</v>
       </c>
@@ -20762,7 +20765,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="87" t="str">
         <f aca="false">A14</f>
         <v>Ruta en QC</v>
@@ -20842,7 +20845,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W15" s="133" t="n">
+      <c r="W15" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR15)</f>
         <v>10</v>
       </c>
@@ -20903,7 +20906,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="87" t="str">
         <f aca="false">A15</f>
         <v>Ruta en QC</v>
@@ -20983,7 +20986,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W16" s="133" t="n">
+      <c r="W16" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR16)</f>
         <v>10</v>
       </c>
@@ -21044,7 +21047,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="87" t="str">
         <f aca="false">A16</f>
         <v>Ruta en QC</v>
@@ -21124,7 +21127,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W17" s="133" t="n">
+      <c r="W17" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR17)</f>
         <v>10</v>
       </c>
@@ -21185,7 +21188,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="87" t="str">
         <f aca="false">A17</f>
         <v>Ruta en QC</v>
@@ -21265,7 +21268,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W18" s="133" t="n">
+      <c r="W18" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR18)</f>
         <v>10</v>
       </c>
@@ -21326,7 +21329,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="87" t="str">
         <f aca="false">A18</f>
         <v>Ruta en QC</v>
@@ -21406,7 +21409,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W19" s="133" t="n">
+      <c r="W19" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR19)</f>
         <v>10</v>
       </c>
@@ -21467,7 +21470,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="87" t="str">
         <f aca="false">A19</f>
         <v>Ruta en QC</v>
@@ -21547,7 +21550,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W20" s="133" t="n">
+      <c r="W20" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR20)</f>
         <v>10</v>
       </c>
@@ -21608,7 +21611,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="87" t="str">
         <f aca="false">A20</f>
         <v>Ruta en QC</v>
@@ -21688,7 +21691,7 @@
 Nivel de confianza: Confirmado
 (AV:N/AC:L/Au:N/C:C/I:C/A:C/E:H/RL:U/RC:C)</v>
       </c>
-      <c r="W21" s="133" t="n">
+      <c r="W21" s="135" t="n">
         <f aca="true">INDIRECT("Hallazgos!H"&amp;AR21)</f>
         <v>10</v>
       </c>
@@ -21749,7 +21752,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="87" t="str">
         <f aca="false">A21</f>
         <v>Ruta en QC</v>
@@ -21882,7 +21885,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="87" t="str">
         <f aca="false">A22</f>
         <v>Ruta en QC</v>
@@ -22015,7 +22018,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="87" t="str">
         <f aca="false">A23</f>
         <v>Ruta en QC</v>
@@ -22148,7 +22151,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="87" t="str">
         <f aca="false">A24</f>
         <v>Ruta en QC</v>
@@ -22281,7 +22284,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="87" t="str">
         <f aca="false">A25</f>
         <v>Ruta en QC</v>
@@ -22414,7 +22417,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="87" t="str">
         <f aca="false">A26</f>
         <v>Ruta en QC</v>
@@ -22547,7 +22550,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="87" t="str">
         <f aca="false">A27</f>
         <v>Ruta en QC</v>
@@ -22680,7 +22683,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="87" t="str">
         <f aca="false">A28</f>
         <v>Ruta en QC</v>
@@ -22813,7 +22816,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="87" t="str">
         <f aca="false">A29</f>
         <v>Ruta en QC</v>
@@ -22946,7 +22949,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="87" t="str">
         <f aca="false">A30</f>
         <v>Ruta en QC</v>
@@ -23176,9 +23179,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="51.5663265306123"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="50.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23433,10 +23436,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23573,12 +23576,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23862,12 +23865,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.2193877551021"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24117,18 +24120,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.9693877551021"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.5408163265306"/>
     <col collapsed="false" hidden="true" max="11" min="11" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35179,27 +35182,26 @@
   </sheetPr>
   <dimension ref="A1:O192"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40473,15 +40475,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="81.5357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="47.7857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.5918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="47.1122448979592"/>
     <col collapsed="false" hidden="true" max="12" min="12" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49566,15 +49568,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="80.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="66.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.9132653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="66.280612244898"/>
     <col collapsed="false" hidden="true" max="8" min="8" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>